<commit_message>
Zeiterfassung_Jeckle_Lukas.xlsx: Neue Zeitposten gebucht.
</commit_message>
<xml_diff>
--- a/1. Projektplanung und Dokumentation/1.1 Zeiterfassung/Zeiterfassung_Jeckle_Lukas.xlsx
+++ b/1. Projektplanung und Dokumentation/1.1 Zeiterfassung/Zeiterfassung_Jeckle_Lukas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://thude0-my.sharepoint.com/personal/jecklu01_hs-ulm_de/Documents/5. Semester/Software Projekt/RaytRazor/1. Projektplanung/1.1 Zeiterfassung/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukas\Desktop\RaytRazor\1. Projektplanung und Dokumentation\1.1 Zeiterfassung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="522" documentId="8_{C9F7BCB0-AC8D-48EA-AB1C-78C940CB4F06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A3CBC778-9DF3-43D3-B51C-F3CC84215839}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524F3EE8-D52E-48C5-B4C4-CCCEBED564D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="630" yWindow="765" windowWidth="28800" windowHeight="15345" xr2:uid="{60F36677-6C43-442F-912E-D347C7303937}"/>
+    <workbookView xWindow="-28920" yWindow="5190" windowWidth="29040" windowHeight="15720" xr2:uid="{60F36677-6C43-442F-912E-D347C7303937}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeiterfassung" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="82">
   <si>
     <t>Name:</t>
   </si>
@@ -260,9 +260,6 @@
     <t>Projektplanung (Product-Backlog, Sprint-Backlogs, Weekly Summaries, …) nachgetragen/aktualisiert und offene TODOs festgehalten</t>
   </si>
   <si>
-    <t>3D-Preview debugging um herauszufinden, wieso Objekte falsch angezeigt werden (ab ~21 Uhr - 00:00 Uhr)</t>
-  </si>
-  <si>
     <t>3D-Preview debugging um falsch angezeigte Objekte richtig und in Farbe dargestellt zu bekommen</t>
   </si>
   <si>
@@ -272,7 +269,19 @@
     <t>Erfahrungsbericht angefangen und Summup für diese Woche erstellt.</t>
   </si>
   <si>
-    <t>Geholfen, Raytracing Schnittstelle in der 3D-Preview zu finalisieren.</t>
+    <t>3D-Preview debugging um herauszufinden, wieso Objekte falsch angezeigt werden</t>
+  </si>
+  <si>
+    <t>Verschiedenste Coding-Unterstützungsarbeiten am Projekt (Coding, Debugging, Mann-für-alle-Fälle, Entscheidungsfindung)</t>
+  </si>
+  <si>
+    <t>GitHub Wiki-Page finalisiert</t>
+  </si>
+  <si>
+    <t>Erfahrungsbericht fertiggestellt</t>
+  </si>
+  <si>
+    <t>Projekt-Abschluss Präsentationen fertiggestellt</t>
   </si>
 </sst>
 </file>
@@ -383,10 +392,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -647,10 +652,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBB1BBFA-3617-4C66-8A60-3FE210797165}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A68" sqref="A68"/>
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1503,7 +1508,7 @@
         <v>12</v>
       </c>
       <c r="D63" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1517,7 +1522,7 @@
         <v>30</v>
       </c>
       <c r="D64" s="7" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1531,7 +1536,7 @@
         <v>30</v>
       </c>
       <c r="D65" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1545,7 +1550,7 @@
         <v>12</v>
       </c>
       <c r="D66" s="7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1553,7 +1558,7 @@
         <v>45678</v>
       </c>
       <c r="B67" s="2">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C67" s="7" t="s">
         <v>30</v>
@@ -1563,31 +1568,68 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="4"/>
-      <c r="C68" s="7"/>
-      <c r="D68" s="7"/>
+      <c r="A68" s="4">
+        <v>45679</v>
+      </c>
+      <c r="B68" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="C68" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>79</v>
+      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="4"/>
+      <c r="A69" s="4">
+        <v>45679</v>
+      </c>
+      <c r="B69" s="2">
+        <v>2</v>
+      </c>
+      <c r="C69" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="4">
+        <v>45679</v>
+      </c>
+      <c r="B70" s="2">
+        <v>4</v>
+      </c>
+      <c r="C70" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="4">
         <v>45314</v>
       </c>
-      <c r="C70" t="s">
+      <c r="B71" s="2">
+        <v>4.5</v>
+      </c>
+      <c r="C71" t="s">
         <v>40</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="2" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="B72" s="2">
-        <f>SUM(B7:B70)</f>
-        <v>140</v>
+      <c r="B73" s="2">
+        <f>SUM(B7:B71)</f>
+        <v>160</v>
       </c>
     </row>
   </sheetData>
@@ -1599,21 +1641,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100EA32FAADEF28B246BE81F09370D9BDD6" ma:contentTypeVersion="4" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="ee5e8cab159ec08823d71aeff920ea58">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="bcfc458b-b0e2-47b4-8909-d39697dfebcc" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="6553d0449cd115c0021964cc0df6b6b1" ns2:_="">
     <xsd:import namespace="bcfc458b-b0e2-47b4-8909-d39697dfebcc"/>
@@ -1757,7 +1784,40 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17D4C286-40F8-430F-9A60-A6D20F13F078}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="bcfc458b-b0e2-47b4-8909-d39697dfebcc"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3F563E5B-E833-4685-AA5F-417D9097CE12}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
@@ -1773,28 +1833,10 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F73990B7-24D7-4B3D-A03A-D9C83C8BF00B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{17D4C286-40F8-430F-9A60-A6D20F13F078}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="bcfc458b-b0e2-47b4-8909-d39697dfebcc"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>